<commit_message>
fixed : datasets and variables order based on dataset type
</commit_message>
<xml_diff>
--- a/data/db_source/dataset.xlsx
+++ b/data/db_source/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBB1906-2D30-5146-A497-AFD9E6C09D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CF95DB-3D78-324E-BB73-9E3FC5C66695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="136">
   <si>
     <t>id</t>
   </si>
@@ -380,6 +380,54 @@
   </si>
   <si>
     <t>anonymous_data, population, culture</t>
+  </si>
+  <si>
+    <t>14-sante</t>
+  </si>
+  <si>
+    <t>04-economie</t>
+  </si>
+  <si>
+    <t>01-pop</t>
+  </si>
+  <si>
+    <t>03-travail</t>
+  </si>
+  <si>
+    <t>08-energie</t>
+  </si>
+  <si>
+    <t>12-monnaie</t>
+  </si>
+  <si>
+    <t>06-industrie</t>
+  </si>
+  <si>
+    <t>11-mobilite</t>
+  </si>
+  <si>
+    <t>10-tourisme</t>
+  </si>
+  <si>
+    <t>02-espace</t>
+  </si>
+  <si>
+    <t>17-politique</t>
+  </si>
+  <si>
+    <t>ofs-salaire</t>
+  </si>
+  <si>
+    <t>ofs-travail</t>
+  </si>
+  <si>
+    <t>ofs</t>
+  </si>
+  <si>
+    <t>ofs-tourisme</t>
+  </si>
+  <si>
+    <t>ofs-div-pop</t>
   </si>
 </sst>
 </file>
@@ -771,10 +819,10 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -783,7 +831,7 @@
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
@@ -859,6 +907,9 @@
       <c r="A2" t="s">
         <v>30</v>
       </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
       <c r="E2" t="s">
         <v>24</v>
       </c>
@@ -891,6 +942,9 @@
       <c r="A3" t="s">
         <v>33</v>
       </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
       <c r="E3" t="s">
         <v>32</v>
       </c>
@@ -931,6 +985,9 @@
     <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
       </c>
       <c r="E4" t="s">
         <v>37</v>
@@ -969,6 +1026,9 @@
       <c r="A5" t="s">
         <v>41</v>
       </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
       <c r="E5" t="s">
         <v>40</v>
       </c>
@@ -994,6 +1054,15 @@
       <c r="A6" t="s">
         <v>43</v>
       </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" t="s">
+        <v>135</v>
+      </c>
       <c r="E6" t="s">
         <v>44</v>
       </c>
@@ -1029,6 +1098,9 @@
       <c r="A7" t="s">
         <v>49</v>
       </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
       <c r="E7" t="s">
         <v>50</v>
       </c>
@@ -1061,6 +1133,9 @@
       <c r="A8" t="s">
         <v>54</v>
       </c>
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
       <c r="E8" t="s">
         <v>55</v>
       </c>
@@ -1096,6 +1171,15 @@
       <c r="A9" t="s">
         <v>60</v>
       </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" t="s">
+        <v>134</v>
+      </c>
       <c r="E9" t="s">
         <v>61</v>
       </c>
@@ -1131,6 +1215,9 @@
       <c r="A10" t="s">
         <v>66</v>
       </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
       <c r="E10" t="s">
         <v>67</v>
       </c>
@@ -1166,6 +1253,9 @@
       <c r="A11" t="s">
         <v>73</v>
       </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
       <c r="E11" t="s">
         <v>74</v>
       </c>
@@ -1201,6 +1291,9 @@
       <c r="A12" t="s">
         <v>78</v>
       </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
       <c r="E12" t="s">
         <v>79</v>
       </c>
@@ -1239,6 +1332,9 @@
       <c r="A13" t="s">
         <v>82</v>
       </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
       <c r="E13" t="s">
         <v>83</v>
       </c>
@@ -1274,6 +1370,9 @@
       <c r="A14" t="s">
         <v>87</v>
       </c>
+      <c r="B14" t="s">
+        <v>120</v>
+      </c>
       <c r="E14" t="s">
         <v>88</v>
       </c>
@@ -1309,6 +1408,9 @@
       <c r="A15" t="s">
         <v>91</v>
       </c>
+      <c r="B15" t="s">
+        <v>127</v>
+      </c>
       <c r="E15" t="s">
         <v>92</v>
       </c>
@@ -1344,6 +1446,9 @@
       <c r="A16" t="s">
         <v>95</v>
       </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
       <c r="E16" t="s">
         <v>96</v>
       </c>
@@ -1379,6 +1484,9 @@
       <c r="A17" t="s">
         <v>99</v>
       </c>
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
       <c r="E17" t="s">
         <v>100</v>
       </c>
@@ -1414,6 +1522,9 @@
       <c r="A18" t="s">
         <v>103</v>
       </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
       <c r="E18" t="s">
         <v>104</v>
       </c>
@@ -1449,6 +1560,15 @@
       <c r="A19" t="s">
         <v>106</v>
       </c>
+      <c r="B19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" t="s">
+        <v>131</v>
+      </c>
       <c r="E19" t="s">
         <v>107</v>
       </c>
@@ -1483,6 +1603,15 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>110</v>
+      </c>
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
       </c>
       <c r="E20" t="s">
         <v>111</v>

</xml_diff>

<commit_message>
fixed : internal link changing param but same page
</commit_message>
<xml_diff>
--- a/data/db_source/dataset.xlsx
+++ b/data/db_source/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777B211D-D6B3-F343-A6D1-7AC9113C5EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4726EDAE-BD0D-5049-8ABB-889AA8FF8971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="143">
   <si>
     <t>id</t>
   </si>
@@ -331,9 +331,6 @@
     <t>emploi_jeunes</t>
   </si>
   <si>
-    <t>Taux d’emploi des jeunes</t>
-  </si>
-  <si>
     <t>Données sur l’emploi des jeunes de 18 à 25 ans</t>
   </si>
   <si>
@@ -443,6 +440,15 @@
   </si>
   <si>
     <t>Évolution des emplois de la tech</t>
+  </si>
+  <si>
+    <t>archived</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Taux d’emploi des jeunes et des moins jeunes</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -518,9 +527,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:R20" totalsRowShown="0">
-  <autoFilter ref="A1:R20" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:S20" totalsRowShown="0">
+  <autoFilter ref="A1:S20" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
+  <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{080E2F00-A22C-534D-B9C4-D8C8D5EB31DA}" name="id"/>
     <tableColumn id="2" xr3:uid="{92BFA972-4C1D-4E43-B990-63C7415BF3D0}" name="folder_id"/>
     <tableColumn id="3" xr3:uid="{39D90AAB-DB99-4842-B7A2-ED8697C478CE}" name="owner_id"/>
@@ -529,10 +538,11 @@
     <tableColumn id="6" xr3:uid="{D2392623-916B-E04B-A27E-0D01B8B20172}" name="type"/>
     <tableColumn id="7" xr3:uid="{4D4990DC-E580-924E-A6C8-71E0E49DC440}" name="description"/>
     <tableColumn id="8" xr3:uid="{489A14B1-8FC8-C549-8AE1-29C457B8AA01}" name="nb_row"/>
-    <tableColumn id="11" xr3:uid="{39B5740A-29A3-4149-AEFD-550E62863529}" name="last_update_date" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{39B5740A-29A3-4149-AEFD-550E62863529}" name="last_update_date" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{40840879-BBAB-7248-8755-9023914314E8}" name="archived" dataDxfId="0"/>
     <tableColumn id="12" xr3:uid="{25BA5CC3-7EA6-8F48-BADD-686749A186ED}" name="updating_each"/>
-    <tableColumn id="13" xr3:uid="{48FD3A95-5D63-5842-ADE8-82D53CC7CB3B}" name="start_date" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{E9CC3D9F-3681-CE44-9463-02B41A65AEDA}" name="end_date" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{48FD3A95-5D63-5842-ADE8-82D53CC7CB3B}" name="start_date" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{E9CC3D9F-3681-CE44-9463-02B41A65AEDA}" name="end_date" dataDxfId="1"/>
     <tableColumn id="9" xr3:uid="{AB83C6F1-9210-B442-AD5A-A3BA93064343}" name="localisation"/>
     <tableColumn id="16" xr3:uid="{ED3587E2-4956-D94E-81CF-A84E6EFAC119}" name="delivery_format"/>
     <tableColumn id="14" xr3:uid="{7536954D-F305-F647-B54D-43D736B0B7C6}" name="link"/>
@@ -831,13 +841,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -851,18 +861,19 @@
     <col min="7" max="7" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" customWidth="1"/>
-    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -890,46 +901,49 @@
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
-        <v>109</v>
-      </c>
       <c r="R1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="S1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
         <v>125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>126</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -943,34 +957,34 @@
       <c r="H2">
         <v>3000</v>
       </c>
-      <c r="J2" t="s">
-        <v>134</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="K2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" s="1">
         <v>2002</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>2023</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>27</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
@@ -987,40 +1001,43 @@
       <c r="I3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J3" t="s">
-        <v>134</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K3" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>21</v>
-      </c>
-      <c r="O3" t="s">
-        <v>14</v>
       </c>
       <c r="P3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="Q3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
@@ -1037,30 +1054,30 @@
       <c r="I4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J4" t="s">
-        <v>135</v>
-      </c>
-      <c r="K4" s="1"/>
+      <c r="K4" t="s">
+        <v>134</v>
+      </c>
       <c r="L4" s="1"/>
-      <c r="M4" t="s">
+      <c r="M4" s="1"/>
+      <c r="N4" t="s">
         <v>25</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="R4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
@@ -1069,32 +1086,32 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H5">
         <v>200</v>
       </c>
-      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" t="s">
+      <c r="M5" s="1"/>
+      <c r="N5" t="s">
         <v>27</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
         <v>41</v>
@@ -1103,7 +1120,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H6">
         <v>500000</v>
@@ -1111,28 +1128,28 @@
       <c r="I6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J6" t="s">
-        <v>134</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" t="s">
+        <v>133</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>26</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>
@@ -1146,28 +1163,31 @@
       <c r="I7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J7" t="s">
-        <v>135</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="J7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K7" t="s">
+        <v>134</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>25</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
         <v>51</v>
@@ -1184,34 +1204,34 @@
       <c r="I8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J8" t="s">
-        <v>134</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" t="s">
+        <v>133</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>66</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" t="s">
         <v>125</v>
-      </c>
-      <c r="D9" t="s">
-        <v>126</v>
       </c>
       <c r="E9" t="s">
         <v>57</v>
@@ -1228,28 +1248,28 @@
       <c r="I9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J9" t="s">
-        <v>136</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" t="s">
+        <v>135</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>26</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E10" t="s">
         <v>62</v>
@@ -1266,28 +1286,28 @@
       <c r="I10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J10" t="s">
-        <v>135</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" t="s">
+        <v>134</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>67</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E11" t="s">
         <v>69</v>
@@ -1296,7 +1316,7 @@
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H11">
         <v>90000</v>
@@ -1304,28 +1324,28 @@
       <c r="I11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J11" t="s">
-        <v>135</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" t="s">
+        <v>134</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>27</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E12" t="s">
         <v>73</v>
@@ -1342,34 +1362,34 @@
       <c r="I12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J12" t="s">
-        <v>134</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" t="s">
+        <v>133</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="M12" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="N12" t="s">
         <v>26</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>39</v>
       </c>
-      <c r="Q12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
@@ -1383,28 +1403,28 @@
       <c r="I13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J13" t="s">
-        <v>136</v>
-      </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" t="s">
+        <v>135</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M13" t="s">
+      <c r="M13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N13" t="s">
         <v>25</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E14" t="s">
         <v>81</v>
@@ -1421,28 +1441,28 @@
       <c r="I14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J14" t="s">
-        <v>134</v>
-      </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" t="s">
+        <v>133</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>27</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E15" t="s">
         <v>85</v>
@@ -1459,28 +1479,28 @@
       <c r="I15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J15" t="s">
-        <v>136</v>
-      </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" t="s">
+        <v>135</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>26</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E16" t="s">
         <v>89</v>
@@ -1497,28 +1517,28 @@
       <c r="I16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J16" t="s">
-        <v>135</v>
-      </c>
-      <c r="K16" s="1" t="s">
+      <c r="K16" t="s">
+        <v>134</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>25</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E17" t="s">
         <v>93</v>
@@ -1527,7 +1547,7 @@
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H17">
         <v>100000</v>
@@ -1535,28 +1555,28 @@
       <c r="I17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J17" t="s">
-        <v>137</v>
-      </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" t="s">
+        <v>136</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>66</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>95</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E18" t="s">
         <v>96</v>
@@ -1573,34 +1593,34 @@
       <c r="I18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J18" t="s">
-        <v>135</v>
-      </c>
-      <c r="K18" s="1" t="s">
+      <c r="K18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>26</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E19" t="s">
         <v>99</v>
@@ -1617,75 +1637,75 @@
       <c r="I19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J19" t="s">
-        <v>134</v>
-      </c>
-      <c r="K19" s="1" t="s">
+      <c r="K19" t="s">
+        <v>133</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>67</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H20">
         <v>100000</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K20" t="s">
+        <v>135</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J20" t="s">
-        <v>136</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>27</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" t="s">
         <v>139</v>
-      </c>
-      <c r="B21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" t="s">
-        <v>140</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
@@ -1699,19 +1719,19 @@
       <c r="I21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J21" t="s">
-        <v>136</v>
-      </c>
-      <c r="K21" s="1" t="s">
+      <c r="K21" t="s">
+        <v>135</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M21" t="s">
+      <c r="M21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N21" t="s">
         <v>25</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added : entity color on links hover or active, evolution diff for number and date relative, changed : doc last update date use Column.timestamp()
</commit_message>
<xml_diff>
--- a/data/db_source/dataset.xlsx
+++ b/data/db_source/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BA43AA-9E06-BF4F-AB57-C030204CDDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9E3340-9F9F-3543-975E-308420C62B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="144">
   <si>
     <t>id</t>
   </si>
@@ -325,9 +325,6 @@
     <t>Étude sur les revenus des ménages suisses</t>
   </si>
   <si>
-    <t>2024/06/30</t>
-  </si>
-  <si>
     <t>emploi_jeunes</t>
   </si>
   <si>
@@ -449,6 +446,12 @@
   </si>
   <si>
     <t>no_more_update</t>
+  </si>
+  <si>
+    <t>2025/01/19</t>
+  </si>
+  <si>
+    <t>2024/05/30</t>
   </si>
 </sst>
 </file>
@@ -844,10 +847,10 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -901,7 +904,7 @@
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
@@ -925,10 +928,10 @@
         <v>19</v>
       </c>
       <c r="R1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -936,13 +939,13 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
         <v>124</v>
-      </c>
-      <c r="D2" t="s">
-        <v>125</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -957,7 +960,7 @@
         <v>3000</v>
       </c>
       <c r="K2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L2" s="1">
         <v>2002</v>
@@ -977,13 +980,13 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
@@ -1001,10 +1004,10 @@
         <v>34</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>17</v>
@@ -1030,13 +1033,13 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
@@ -1054,7 +1057,7 @@
         <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1065,10 +1068,10 @@
         <v>22</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1076,7 +1079,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
@@ -1085,7 +1088,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H5">
         <v>200</v>
@@ -1104,13 +1107,13 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E6" t="s">
         <v>41</v>
@@ -1119,7 +1122,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H6">
         <v>500000</v>
@@ -1128,7 +1131,7 @@
         <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>43</v>
@@ -1148,7 +1151,7 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>
@@ -1163,10 +1166,10 @@
         <v>48</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>49</v>
@@ -1186,7 +1189,7 @@
         <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
         <v>51</v>
@@ -1204,7 +1207,7 @@
         <v>53</v>
       </c>
       <c r="K8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>54</v>
@@ -1224,13 +1227,13 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
         <v>124</v>
-      </c>
-      <c r="D9" t="s">
-        <v>125</v>
       </c>
       <c r="E9" t="s">
         <v>57</v>
@@ -1248,7 +1251,7 @@
         <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>60</v>
@@ -1268,7 +1271,7 @@
         <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E10" t="s">
         <v>62</v>
@@ -1286,7 +1289,7 @@
         <v>64</v>
       </c>
       <c r="K10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>65</v>
@@ -1306,7 +1309,7 @@
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E11" t="s">
         <v>69</v>
@@ -1315,7 +1318,7 @@
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H11">
         <v>90000</v>
@@ -1324,7 +1327,7 @@
         <v>70</v>
       </c>
       <c r="K11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>71</v>
@@ -1344,7 +1347,7 @@
         <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E12" t="s">
         <v>73</v>
@@ -1362,13 +1365,13 @@
         <v>75</v>
       </c>
       <c r="K12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>60</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N12" t="s">
         <v>26</v>
@@ -1377,7 +1380,7 @@
         <v>39</v>
       </c>
       <c r="R12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
@@ -1385,10 +1388,10 @@
         <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
@@ -1403,13 +1406,13 @@
         <v>78</v>
       </c>
       <c r="K13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N13" t="s">
         <v>25</v>
@@ -1423,7 +1426,7 @@
         <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14" t="s">
         <v>81</v>
@@ -1441,7 +1444,7 @@
         <v>83</v>
       </c>
       <c r="K14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>54</v>
@@ -1461,7 +1464,7 @@
         <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15" t="s">
         <v>85</v>
@@ -1479,7 +1482,7 @@
         <v>87</v>
       </c>
       <c r="K15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>71</v>
@@ -1499,7 +1502,7 @@
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E16" t="s">
         <v>89</v>
@@ -1517,7 +1520,7 @@
         <v>91</v>
       </c>
       <c r="K16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>60</v>
@@ -1537,7 +1540,7 @@
         <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E17" t="s">
         <v>93</v>
@@ -1546,7 +1549,7 @@
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H17">
         <v>100000</v>
@@ -1555,7 +1558,7 @@
         <v>94</v>
       </c>
       <c r="K17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>54</v>
@@ -1575,7 +1578,7 @@
         <v>95</v>
       </c>
       <c r="B18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E18" t="s">
         <v>96</v>
@@ -1593,7 +1596,7 @@
         <v>70</v>
       </c>
       <c r="K18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>60</v>
@@ -1613,13 +1616,13 @@
         <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E19" t="s">
         <v>99</v>
@@ -1631,13 +1634,13 @@
         <v>100</v>
       </c>
       <c r="H19">
-        <v>45000</v>
+        <v>46000</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="K19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>54</v>
@@ -1654,37 +1657,37 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H20">
         <v>100000</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K20" t="s">
+        <v>134</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="K20" t="s">
-        <v>135</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>44</v>
@@ -1698,13 +1701,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" t="s">
         <v>138</v>
-      </c>
-      <c r="B21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" t="s">
-        <v>139</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
@@ -1716,16 +1719,16 @@
         <v>200000</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>78</v>
+        <v>142</v>
       </c>
       <c r="K21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N21" t="s">
         <v>25</v>

</xml_diff>